<commit_message>
Tätigkeitsliste hinzugefügt, Zeitplan angepasst
</commit_message>
<xml_diff>
--- a/LB306_Dokumente/Zeitplan/Zeitplan ZNRGT.xlsx
+++ b/LB306_Dokumente/Zeitplan/Zeitplan ZNRGT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbbaden-my.sharepoint.com/personal/a_niklaus_inf21_stud_bbbaden_ch/Documents/Dokumente/GitHub/Built-different-ATM/LB306_Dokumente/Zeitplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8673DA0-ECE4-440C-A7B2-504492AE797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{C8673DA0-ECE4-440C-A7B2-504492AE797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D01447D-B027-4B51-A004-654250ABFCF8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D70A4009-B28E-40A2-975C-C0AC8919D4C8}"/>
   </bookViews>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56094ED0-7023-43B3-AF69-D143D07D2D6D}">
   <dimension ref="A1:AP55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,7 +1195,7 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="O17" s="2"/>
-      <c r="T17" s="2"/>
+      <c r="T17" s="36"/>
       <c r="X17" s="18"/>
       <c r="AD17" s="2"/>
       <c r="AI17" s="2"/>
@@ -1261,6 +1261,8 @@
       <c r="D21" s="1"/>
       <c r="J21" s="2"/>
       <c r="O21" s="2"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
       <c r="T21" s="2"/>
       <c r="X21" s="18"/>
       <c r="AD21" s="2"/>

</xml_diff>

<commit_message>
Auswerten und Zeitplanung aktualisiert
</commit_message>
<xml_diff>
--- a/LB306_Dokumente/Zeitplan/Zeitplan ZNRGT.xlsx
+++ b/LB306_Dokumente/Zeitplan/Zeitplan ZNRGT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbbaden-my.sharepoint.com/personal/a_niklaus_inf21_stud_bbbaden_ch/Documents/Dokumente/GitHub/Built-different-ATM/LB306_Dokumente/Zeitplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{C8673DA0-ECE4-440C-A7B2-504492AE797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B59A55D-53E2-4485-9909-AC851CB2CB01}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{C8673DA0-ECE4-440C-A7B2-504492AE797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49D098AC-BDE1-4C74-9347-8BCDA1541F16}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D70A4009-B28E-40A2-975C-C0AC8919D4C8}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -442,36 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -487,9 +458,36 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -806,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56094ED0-7023-43B3-AF69-D143D07D2D6D}">
   <dimension ref="A1:AP55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE35" sqref="AE35"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,61 +830,61 @@
     </row>
     <row r="2" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:42" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="32"/>
-      <c r="E3" s="46">
+      <c r="E3" s="48">
         <v>44915</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="44">
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="46">
         <v>44936</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="44">
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="46">
         <v>44943</v>
       </c>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="44">
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="46">
         <v>44950</v>
       </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="44">
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="46">
         <v>44957</v>
       </c>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="44">
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="46">
         <v>44978</v>
       </c>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="46"/>
-      <c r="AG3" s="46"/>
-      <c r="AH3" s="46"/>
-      <c r="AI3" s="44">
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="46">
         <v>44985</v>
       </c>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="45"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="46"/>
+      <c r="AM3" s="47"/>
     </row>
     <row r="4" spans="1:42" s="8" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
@@ -930,13 +928,13 @@
       <c r="AM4" s="17"/>
     </row>
     <row r="5" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="45">
         <v>1</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1"/>
@@ -954,9 +952,9 @@
       <c r="AM5" s="18"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="1"/>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
@@ -973,11 +971,11 @@
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="42">
+      <c r="A7" s="39"/>
+      <c r="B7" s="45">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
@@ -997,9 +995,9 @@
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="41"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="1"/>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
@@ -1016,11 +1014,11 @@
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="42">
+      <c r="A9" s="39"/>
+      <c r="B9" s="45">
         <v>1.2</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="44" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1"/>
@@ -1040,9 +1038,9 @@
       <c r="AM9" s="18"/>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="41"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="1"/>
       <c r="J10" s="34"/>
       <c r="K10" s="33"/>
@@ -1056,11 +1054,11 @@
       <c r="AM10" s="18"/>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="42">
+      <c r="A11" s="39"/>
+      <c r="B11" s="45">
         <v>1.3</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="50" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1"/>
@@ -1074,9 +1072,9 @@
       <c r="AM11" s="18"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="38"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="1"/>
       <c r="J12" s="2"/>
       <c r="M12" s="33"/>
@@ -1091,11 +1089,11 @@
       <c r="AM12" s="18"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="42">
+      <c r="A13" s="39"/>
+      <c r="B13" s="45">
         <v>1.4</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="50" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="1"/>
@@ -1114,9 +1112,9 @@
       <c r="AM13" s="18"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="38"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="1"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
@@ -1170,13 +1168,13 @@
       <c r="AM15" s="22"/>
     </row>
     <row r="16" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="45">
         <v>2</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="50" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1"/>
@@ -1197,9 +1195,9 @@
       <c r="AM16" s="18"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="38"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="1"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
@@ -1219,11 +1217,11 @@
       <c r="AM17" s="18"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="42">
+      <c r="A18" s="39"/>
+      <c r="B18" s="45">
         <v>2.1</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="1"/>
@@ -1238,9 +1236,9 @@
       <c r="AM18" s="18"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="38"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="1"/>
       <c r="J19" s="2"/>
       <c r="O19" s="2"/>
@@ -1253,11 +1251,11 @@
       <c r="AM19" s="18"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
-      <c r="B20" s="42">
+      <c r="A20" s="39"/>
+      <c r="B20" s="45">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="1"/>
@@ -1272,9 +1270,9 @@
       <c r="AM20" s="18"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="38"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="1"/>
       <c r="J21" s="2"/>
       <c r="O21" s="2"/>
@@ -1329,13 +1327,13 @@
       <c r="AM22" s="22"/>
     </row>
     <row r="23" spans="1:39" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="45">
         <v>3</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="50" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="1"/>
@@ -1348,9 +1346,9 @@
       <c r="AM23" s="18"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="38"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="1"/>
       <c r="J24" s="2"/>
       <c r="O24" s="2"/>
@@ -1404,13 +1402,13 @@
       <c r="AM25" s="22"/>
     </row>
     <row r="26" spans="1:39" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="42">
+      <c r="B26" s="45">
         <v>4</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="44" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="1"/>
@@ -1433,9 +1431,9 @@
       <c r="AM26" s="18"/>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A27" s="48"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="41"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="1"/>
       <c r="J27" s="2"/>
       <c r="O27" s="2"/>
@@ -1498,13 +1496,13 @@
       <c r="AM28" s="22"/>
     </row>
     <row r="29" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29" s="45">
         <v>5</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="50" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="1"/>
@@ -1518,26 +1516,26 @@
       <c r="AM29" s="18"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="38"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="1"/>
       <c r="J30" s="2"/>
       <c r="O30" s="2"/>
       <c r="T30" s="2"/>
       <c r="X30" s="18"/>
       <c r="AD30" s="2"/>
-      <c r="AH30" s="53"/>
+      <c r="AH30" s="38"/>
       <c r="AI30" s="36"/>
       <c r="AJ30" s="33"/>
       <c r="AM30" s="18"/>
     </row>
     <row r="31" spans="1:39" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48"/>
-      <c r="B31" s="42">
+      <c r="A31" s="39"/>
+      <c r="B31" s="45">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="1"/>
@@ -1551,9 +1549,9 @@
       <c r="AM31" s="18"/>
     </row>
     <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="48"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="38"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="1"/>
       <c r="J32" s="2"/>
       <c r="O32" s="2"/>
@@ -1606,13 +1604,13 @@
       <c r="AM33" s="22"/>
     </row>
     <row r="34" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="42">
+      <c r="B34" s="45">
         <v>6</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="50" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="1"/>
@@ -1626,9 +1624,9 @@
       <c r="AM34" s="18"/>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A35" s="48"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="38"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="1"/>
       <c r="J35" s="2"/>
       <c r="O35" s="2"/>
@@ -1641,11 +1639,11 @@
       <c r="AM35" s="18"/>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A36" s="48"/>
-      <c r="B36" s="42">
+      <c r="A36" s="39"/>
+      <c r="B36" s="45">
         <v>6.1</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="50" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="1"/>
@@ -1659,9 +1657,9 @@
       <c r="AM36" s="18"/>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A37" s="48"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="38"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="1"/>
       <c r="J37" s="2"/>
       <c r="O37" s="2"/>
@@ -1674,11 +1672,11 @@
       <c r="AM37" s="18"/>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A38" s="48"/>
-      <c r="B38" s="42">
+      <c r="A38" s="39"/>
+      <c r="B38" s="45">
         <v>6.2</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="50" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="1"/>
@@ -1692,9 +1690,9 @@
       <c r="AM38" s="18"/>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A39" s="48"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="38"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="1"/>
       <c r="J39" s="2"/>
       <c r="O39" s="2"/>
@@ -1707,11 +1705,11 @@
       <c r="AM39" s="18"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A40" s="48"/>
-      <c r="B40" s="42">
+      <c r="A40" s="39"/>
+      <c r="B40" s="45">
         <v>6.3</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D40" s="1"/>
@@ -1725,9 +1723,9 @@
       <c r="AM40" s="18"/>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A41" s="48"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="38"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="1"/>
       <c r="J41" s="2"/>
       <c r="O41" s="2"/>
@@ -1740,11 +1738,11 @@
       <c r="AM41" s="18"/>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A42" s="48"/>
-      <c r="B42" s="42">
+      <c r="A42" s="39"/>
+      <c r="B42" s="45">
         <v>6.4</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="52" t="s">
         <v>27</v>
       </c>
       <c r="D42" s="1"/>
@@ -1758,9 +1756,9 @@
       <c r="AM42" s="18"/>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A43" s="48"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="40"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="52"/>
       <c r="D43" s="1"/>
       <c r="J43" s="2"/>
       <c r="O43" s="2"/>
@@ -1773,11 +1771,11 @@
       <c r="AM43" s="18"/>
     </row>
     <row r="44" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="48"/>
-      <c r="B44" s="42">
+      <c r="A44" s="39"/>
+      <c r="B44" s="45">
         <v>6.5</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C44" s="50" t="s">
         <v>28</v>
       </c>
       <c r="D44" s="1"/>
@@ -1791,9 +1789,9 @@
       <c r="AM44" s="18"/>
     </row>
     <row r="45" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="48"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="38"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="1"/>
       <c r="J45" s="2"/>
       <c r="O45" s="2"/>
@@ -1847,13 +1845,13 @@
       <c r="AM46" s="22"/>
     </row>
     <row r="47" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="42">
+      <c r="B47" s="45">
         <v>7</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="50" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="1"/>
@@ -1894,9 +1892,9 @@
       <c r="AM47" s="31"/>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="38"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="1"/>
       <c r="J48" s="2"/>
       <c r="O48" s="2"/>
@@ -1908,11 +1906,11 @@
       <c r="AM48" s="18"/>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A49" s="50"/>
-      <c r="B49" s="42">
+      <c r="A49" s="41"/>
+      <c r="B49" s="45">
         <v>7.1</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="50" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="1"/>
@@ -1930,9 +1928,9 @@
       <c r="AM49" s="31"/>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A50" s="50"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="38"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="1"/>
       <c r="J50" s="2"/>
       <c r="N50" s="35"/>
@@ -1987,13 +1985,13 @@
       <c r="AM51" s="22"/>
     </row>
     <row r="52" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="42">
+      <c r="B52" s="45">
         <v>8</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="50" t="s">
         <v>33</v>
       </c>
       <c r="D52" s="1"/>
@@ -2008,9 +2006,9 @@
       <c r="AM52" s="31"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A53" s="50"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="38"/>
+      <c r="A53" s="41"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="1"/>
       <c r="J53" s="2"/>
       <c r="O53" s="2"/>
@@ -2025,11 +2023,11 @@
       <c r="AM53" s="37"/>
     </row>
     <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="50"/>
-      <c r="B54" s="42">
+      <c r="A54" s="41"/>
+      <c r="B54" s="45">
         <v>8.1</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="50" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="1"/>
@@ -2039,14 +2037,13 @@
       <c r="X54" s="18"/>
       <c r="Y54" s="2"/>
       <c r="AD54" s="2"/>
-      <c r="AI54" s="54"/>
-      <c r="AJ54" s="55"/>
+      <c r="AI54" s="2"/>
       <c r="AM54" s="18"/>
     </row>
     <row r="55" spans="1:39" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="51"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="39"/>
+      <c r="A55" s="42"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="53"/>
       <c r="D55" s="21"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -2086,6 +2083,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="AI3:AM3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="Y3:AC3"/>
+    <mergeCell ref="AD3:AH3"/>
     <mergeCell ref="A34:A45"/>
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="A52:A55"/>
@@ -2102,50 +2143,6 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="AI3:AM3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="Y3:AC3"/>
-    <mergeCell ref="AD3:AH3"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>